<commit_message>
Added test for adding a book to user profile
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\IdeaProjects\Bookstore18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E24DDA3-1D82-41AD-9862-CD7977E4C07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F9811E-9AA0-4E0F-B676-0183DC3F3302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Books" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Valid Username</t>
   </si>
@@ -61,13 +62,22 @@
   </si>
   <si>
     <t>982h3t89h0p4</t>
+  </si>
+  <si>
+    <t>dragoljubqa</t>
+  </si>
+  <si>
+    <t>Qwerty123!@#</t>
+  </si>
+  <si>
+    <t>Speaking JavaScript</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +92,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,9 +121,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -391,11 +410,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -403,7 +422,7 @@
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,8 +436,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -426,7 +450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -434,7 +458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -442,12 +466,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CA48295C-E4B1-4B39-A5D1-A872AB5C28DD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B888EE-91FD-496F-BC36-48845A601A0A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>